<commit_message>
Import Excel file functionality added.
</commit_message>
<xml_diff>
--- a/Collection1/ObjetSelection1.xlsx
+++ b/Collection1/ObjetSelection1.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t>Objet ID</t>
   </si>
@@ -29,34 +29,25 @@
     <t>Localisation</t>
   </si>
   <si>
-    <t>183</t>
+    <t>393</t>
   </si>
   <si>
-    <t>Milla en Floride</t>
-  </si>
-  <si>
-    <t>EXPO</t>
-  </si>
-  <si>
-    <t>2011.1.27</t>
-  </si>
-  <si>
-    <t>USA</t>
-  </si>
-  <si>
-    <t>184</t>
-  </si>
-  <si>
-    <t>ffffffffeeee</t>
+    <t>ccccc</t>
   </si>
   <si>
     <t>CEC</t>
   </si>
   <si>
-    <t>ffeeeeee</t>
+    <t>v1987.4.6</t>
   </si>
   <si>
-    <t>ffeeeee</t>
+    <t>B544</t>
+  </si>
+  <si>
+    <t>392</t>
+  </si>
+  <si>
+    <t>vu</t>
   </si>
 </sst>
 </file>
@@ -106,6 +97,12 @@
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="2" max="2" width="12.734375" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="14.47265625" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="9.81640625" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="11.58203125" customWidth="true" bestFit="true"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
@@ -146,16 +143,16 @@
         <v>10</v>
       </c>
       <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Search function added successfully ;)
</commit_message>
<xml_diff>
--- a/Collection1/ObjetSelection1.xlsx
+++ b/Collection1/ObjetSelection1.xlsx
@@ -29,19 +29,19 @@
     <t>Localisation</t>
   </si>
   <si>
-    <t>402</t>
+    <t>413</t>
   </si>
   <si>
-    <t>ccccc</t>
+    <t>bateau</t>
   </si>
   <si>
-    <t>CEC</t>
+    <t>EXPO</t>
   </si>
   <si>
-    <t>v1987.4.6</t>
+    <t>3089.4.6d</t>
   </si>
   <si>
-    <t>B544</t>
+    <t>dddd</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Directory chooser & Alert dialog boxes added.
</commit_message>
<xml_diff>
--- a/Collection1/ObjetSelection1.xlsx
+++ b/Collection1/ObjetSelection1.xlsx
@@ -29,13 +29,13 @@
     <t>Localisation</t>
   </si>
   <si>
-    <t>413</t>
+    <t>422</t>
   </si>
   <si>
-    <t>bateau</t>
+    <t>marteau</t>
   </si>
   <si>
-    <t>EXPO</t>
+    <t>CG04</t>
   </si>
   <si>
     <t>3089.4.6d</t>

</xml_diff>